<commit_message>
Update top_level_task_sheet_schedule_decoupled-V1.xlsx with new data
</commit_message>
<xml_diff>
--- a/artifacts/top_level_task_sheet_schedule_decoupled-V1.xlsx
+++ b/artifacts/top_level_task_sheet_schedule_decoupled-V1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\spring-2025\Compilers\LABs\lab-schedule-decoupled\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9BD435B-5625-4450-BF34-14E8DC386599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A159AF1-0A1A-463E-95C4-9DE99F97BAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -2332,6 +2332,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="20" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2371,7 +2372,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="20" applyFill="1"/>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="% complete" xfId="6" xr:uid="{B0E3096C-C39B-4004-853A-D4C56CDC9555}"/>
@@ -2851,7 +2851,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1FC06A3-543F-4971-A317-96FE7AF52EC7}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -3072,7 +3072,7 @@
       <c r="B11" s="16" t="s">
         <v>373</v>
       </c>
-      <c r="C11" s="80" t="s">
+      <c r="C11" s="67" t="s">
         <v>374</v>
       </c>
       <c r="D11" s="16"/>
@@ -3092,7 +3092,7 @@
       <c r="B13" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="C13" s="80" t="s">
+      <c r="C13" s="67" t="s">
         <v>377</v>
       </c>
       <c r="D13" s="16"/>
@@ -3104,7 +3104,7 @@
       <c r="B14" s="16" t="s">
         <v>378</v>
       </c>
-      <c r="C14" s="80" t="s">
+      <c r="C14" s="67" t="s">
         <v>379</v>
       </c>
       <c r="D14" s="16"/>
@@ -3116,7 +3116,7 @@
       <c r="B15" s="16" t="s">
         <v>380</v>
       </c>
-      <c r="C15" s="80" t="s">
+      <c r="C15" s="67" t="s">
         <v>381</v>
       </c>
       <c r="D15" s="16"/>
@@ -3128,7 +3128,7 @@
       <c r="B16" s="16" t="s">
         <v>382</v>
       </c>
-      <c r="C16" s="80" t="s">
+      <c r="C16" s="67" t="s">
         <v>383</v>
       </c>
       <c r="D16" s="16"/>
@@ -3195,27 +3195,27 @@
       </c>
       <c r="B26" s="23">
         <f>Attendance!C26</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C26" s="23">
         <f>Attendance!D26</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D26" s="23">
         <f>Attendance!E26</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E26" s="23">
         <f>Attendance!F26</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F26" s="23">
         <f>Attendance!G26</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G26" s="23">
         <f>Attendance!H26</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
@@ -3247,27 +3247,27 @@
       </c>
       <c r="B28" s="23">
         <f t="shared" ref="B28:G28" si="0">SUM(B26:B27)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C28" s="23">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D28" s="23">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E28" s="23">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F28" s="23">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G28" s="23">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
@@ -3276,7 +3276,7 @@
       </c>
       <c r="B30" s="23">
         <f>SUM(B28:G28)</f>
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
@@ -3463,8 +3463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D498C59D-E060-40B6-B59A-036A9DD1C81C}">
   <dimension ref="A1:AC152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+    <sheetView topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q87" sqref="Q87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3499,14 +3499,14 @@
       <c r="G1" s="7"/>
       <c r="H1" s="28"/>
       <c r="I1" s="17"/>
-      <c r="J1" s="67" t="s">
+      <c r="J1" s="68" t="s">
         <v>71</v>
       </c>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
       <c r="P1" s="62" t="s">
         <v>176</v>
       </c>
@@ -3963,7 +3963,9 @@
       <c r="R8" s="61">
         <v>45720</v>
       </c>
-      <c r="S8" s="61"/>
+      <c r="S8" s="61">
+        <v>45722</v>
+      </c>
       <c r="T8" s="15">
         <f>DATEDIF(Summary!$B$7,P8,"d")+1</f>
         <v>1</v>
@@ -3976,9 +3978,9 @@
         <f>DATEDIF(Summary!$B$7,R8,"d")+1</f>
         <v>1</v>
       </c>
-      <c r="W8" s="15" t="e">
+      <c r="W8" s="15">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>2</v>
       </c>
       <c r="X8">
         <v>76</v>
@@ -4035,7 +4037,9 @@
       <c r="R9" s="61">
         <v>45720</v>
       </c>
-      <c r="S9" s="61"/>
+      <c r="S9" s="61">
+        <v>45727</v>
+      </c>
       <c r="T9" s="15">
         <f>DATEDIF(Summary!$B$7,P9,"d")+1</f>
         <v>1</v>
@@ -4048,9 +4052,9 @@
         <f>DATEDIF(Summary!$B$7,R9,"d")+1</f>
         <v>1</v>
       </c>
-      <c r="W9" s="15" t="e">
+      <c r="W9" s="15">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>7</v>
       </c>
       <c r="X9">
         <v>77</v>
@@ -4107,7 +4111,9 @@
       <c r="R10" s="61">
         <v>45720</v>
       </c>
-      <c r="S10" s="61"/>
+      <c r="S10" s="61">
+        <v>45727</v>
+      </c>
       <c r="T10" s="15">
         <f>DATEDIF(Summary!$B$7,P10,"d")+1</f>
         <v>1</v>
@@ -4120,9 +4126,9 @@
         <f>DATEDIF(Summary!$B$7,R10,"d")+1</f>
         <v>1</v>
       </c>
-      <c r="W10" s="15" t="e">
+      <c r="W10" s="15">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>7</v>
       </c>
       <c r="X10">
         <v>78</v>
@@ -4179,7 +4185,9 @@
       <c r="R11" s="61">
         <v>45720</v>
       </c>
-      <c r="S11" s="61"/>
+      <c r="S11" s="61">
+        <v>45727</v>
+      </c>
       <c r="T11" s="15">
         <f>DATEDIF(Summary!$B$7,P11,"d")+1</f>
         <v>1</v>
@@ -4192,9 +4200,9 @@
         <f>DATEDIF(Summary!$B$7,R11,"d")+1</f>
         <v>1</v>
       </c>
-      <c r="W11" s="15" t="e">
+      <c r="W11" s="15">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>7</v>
       </c>
       <c r="X11">
         <v>79</v>
@@ -8138,7 +8146,9 @@
       <c r="R73" s="61">
         <v>45720</v>
       </c>
-      <c r="S73" s="61"/>
+      <c r="S73" s="61">
+        <v>45727</v>
+      </c>
       <c r="T73" s="15">
         <f>DATEDIF(Summary!$B$7,P73,"d")+1</f>
         <v>1</v>
@@ -8151,9 +8161,9 @@
         <f>DATEDIF(Summary!$B$7,R73,"d")+1</f>
         <v>1</v>
       </c>
-      <c r="W73" s="15" t="e">
+      <c r="W73" s="15">
         <f t="shared" si="14"/>
-        <v>#NUM!</v>
+        <v>7</v>
       </c>
       <c r="X73">
         <v>141</v>
@@ -8206,7 +8216,9 @@
       <c r="R74" s="61">
         <v>45720</v>
       </c>
-      <c r="S74" s="61"/>
+      <c r="S74" s="61">
+        <v>45727</v>
+      </c>
       <c r="T74" s="15">
         <f>DATEDIF(Summary!$B$7,P74,"d")+1</f>
         <v>1</v>
@@ -8219,9 +8231,9 @@
         <f>DATEDIF(Summary!$B$7,R74,"d")+1</f>
         <v>1</v>
       </c>
-      <c r="W74" s="15" t="e">
+      <c r="W74" s="15">
         <f t="shared" si="14"/>
-        <v>#NUM!</v>
+        <v>7</v>
       </c>
       <c r="X74">
         <v>142</v>
@@ -8274,7 +8286,9 @@
       <c r="R75" s="61">
         <v>45720</v>
       </c>
-      <c r="S75" s="61"/>
+      <c r="S75" s="61">
+        <v>45727</v>
+      </c>
       <c r="T75" s="15">
         <f>DATEDIF(Summary!$B$7,P75,"d")+1</f>
         <v>1</v>
@@ -8287,9 +8301,9 @@
         <f>DATEDIF(Summary!$B$7,R75,"d")+1</f>
         <v>1</v>
       </c>
-      <c r="W75" s="15" t="e">
+      <c r="W75" s="15">
         <f t="shared" si="14"/>
-        <v>#NUM!</v>
+        <v>7</v>
       </c>
       <c r="X75">
         <v>143</v>
@@ -8342,7 +8356,9 @@
       <c r="R76" s="61">
         <v>45720</v>
       </c>
-      <c r="S76" s="61"/>
+      <c r="S76" s="61">
+        <v>45727</v>
+      </c>
       <c r="T76" s="15">
         <f>DATEDIF(Summary!$B$7,P76,"d")+1</f>
         <v>1</v>
@@ -8355,9 +8371,9 @@
         <f>DATEDIF(Summary!$B$7,R76,"d")+1</f>
         <v>1</v>
       </c>
-      <c r="W76" s="15" t="e">
+      <c r="W76" s="15">
         <f t="shared" si="14"/>
-        <v>#NUM!</v>
+        <v>7</v>
       </c>
       <c r="X76">
         <v>144</v>
@@ -8410,7 +8426,9 @@
       <c r="R77" s="61">
         <v>45720</v>
       </c>
-      <c r="S77" s="61"/>
+      <c r="S77" s="61">
+        <v>45727</v>
+      </c>
       <c r="T77" s="15">
         <f>DATEDIF(Summary!$B$7,P77,"d")+1</f>
         <v>1</v>
@@ -8423,9 +8441,9 @@
         <f>DATEDIF(Summary!$B$7,R77,"d")+1</f>
         <v>1</v>
       </c>
-      <c r="W77" s="15" t="e">
+      <c r="W77" s="15">
         <f t="shared" si="14"/>
-        <v>#NUM!</v>
+        <v>7</v>
       </c>
       <c r="X77">
         <v>145</v>
@@ -8478,7 +8496,9 @@
       <c r="R78" s="61">
         <v>45720</v>
       </c>
-      <c r="S78" s="61"/>
+      <c r="S78" s="61">
+        <v>45727</v>
+      </c>
       <c r="T78" s="15">
         <f>DATEDIF(Summary!$B$7,P78,"d")+1</f>
         <v>1</v>
@@ -8491,9 +8511,9 @@
         <f>DATEDIF(Summary!$B$7,R78,"d")+1</f>
         <v>1</v>
       </c>
-      <c r="W78" s="15" t="e">
+      <c r="W78" s="15">
         <f t="shared" si="14"/>
-        <v>#NUM!</v>
+        <v>7</v>
       </c>
       <c r="X78">
         <v>146</v>
@@ -8546,7 +8566,9 @@
       <c r="R79" s="61">
         <v>45720</v>
       </c>
-      <c r="S79" s="61"/>
+      <c r="S79" s="61">
+        <v>45727</v>
+      </c>
       <c r="T79" s="15">
         <f>DATEDIF(Summary!$B$7,P79,"d")+1</f>
         <v>1</v>
@@ -8559,9 +8581,9 @@
         <f>DATEDIF(Summary!$B$7,R79,"d")+1</f>
         <v>1</v>
       </c>
-      <c r="W79" s="15" t="e">
+      <c r="W79" s="15">
         <f t="shared" si="14"/>
-        <v>#NUM!</v>
+        <v>7</v>
       </c>
       <c r="X79">
         <v>147</v>
@@ -8614,7 +8636,9 @@
       <c r="R80" s="61">
         <v>45720</v>
       </c>
-      <c r="S80" s="61"/>
+      <c r="S80" s="61">
+        <v>45727</v>
+      </c>
       <c r="T80" s="15">
         <f>DATEDIF(Summary!$B$7,P80,"d")+1</f>
         <v>1</v>
@@ -8627,9 +8651,9 @@
         <f>DATEDIF(Summary!$B$7,R80,"d")+1</f>
         <v>1</v>
       </c>
-      <c r="W80" s="15" t="e">
+      <c r="W80" s="15">
         <f t="shared" si="14"/>
-        <v>#NUM!</v>
+        <v>7</v>
       </c>
       <c r="X80">
         <v>148</v>
@@ -8682,7 +8706,9 @@
       <c r="R81" s="61">
         <v>45720</v>
       </c>
-      <c r="S81" s="61"/>
+      <c r="S81" s="61">
+        <v>45727</v>
+      </c>
       <c r="T81" s="15">
         <f>DATEDIF(Summary!$B$7,P81,"d")+1</f>
         <v>1</v>
@@ -8695,9 +8721,9 @@
         <f>DATEDIF(Summary!$B$7,R81,"d")+1</f>
         <v>1</v>
       </c>
-      <c r="W81" s="15" t="e">
+      <c r="W81" s="15">
         <f t="shared" si="14"/>
-        <v>#NUM!</v>
+        <v>7</v>
       </c>
       <c r="X81">
         <v>149</v>
@@ -8803,7 +8829,9 @@
         <f>P83+7</f>
         <v>45734</v>
       </c>
-      <c r="R83" s="61"/>
+      <c r="R83" s="61">
+        <v>45727</v>
+      </c>
       <c r="S83" s="61"/>
       <c r="T83" s="15">
         <f>DATEDIF(Summary!$B$7,P83,"d")+1</f>
@@ -8813,13 +8841,13 @@
         <f t="shared" si="13"/>
         <v>7</v>
       </c>
-      <c r="V83" s="15" t="e">
+      <c r="V83" s="15">
         <f>DATEDIF(Summary!$B$7,R83,"d")+1</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="W83" s="15">
+        <v>8</v>
+      </c>
+      <c r="W83" s="15" t="e">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="X83">
         <v>151</v>
@@ -8869,7 +8897,9 @@
         <f>P84+7</f>
         <v>45734</v>
       </c>
-      <c r="R84" s="61"/>
+      <c r="R84" s="61">
+        <v>45727</v>
+      </c>
       <c r="S84" s="61"/>
       <c r="T84" s="15">
         <f>DATEDIF(Summary!$B$7,P84,"d")+1</f>
@@ -8879,13 +8909,13 @@
         <f t="shared" si="13"/>
         <v>7</v>
       </c>
-      <c r="V84" s="15" t="e">
+      <c r="V84" s="15">
         <f>DATEDIF(Summary!$B$7,R84,"d")+1</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="W84" s="15">
+        <v>8</v>
+      </c>
+      <c r="W84" s="15" t="e">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="X84">
         <v>152</v>
@@ -8935,7 +8965,9 @@
         <f>P85+7</f>
         <v>45734</v>
       </c>
-      <c r="R85" s="61"/>
+      <c r="R85" s="61">
+        <v>45727</v>
+      </c>
       <c r="S85" s="61"/>
       <c r="T85" s="15">
         <f>DATEDIF(Summary!$B$7,P85,"d")+1</f>
@@ -8945,13 +8977,13 @@
         <f t="shared" si="13"/>
         <v>7</v>
       </c>
-      <c r="V85" s="15" t="e">
+      <c r="V85" s="15">
         <f>DATEDIF(Summary!$B$7,R85,"d")+1</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="W85" s="15">
+        <v>8</v>
+      </c>
+      <c r="W85" s="15" t="e">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="X85">
         <v>153</v>
@@ -9001,7 +9033,9 @@
         <f>P86+7</f>
         <v>45734</v>
       </c>
-      <c r="R86" s="61"/>
+      <c r="R86" s="61">
+        <v>45727</v>
+      </c>
       <c r="S86" s="61"/>
       <c r="T86" s="15">
         <f>DATEDIF(Summary!$B$7,P86,"d")+1</f>
@@ -9011,13 +9045,13 @@
         <f t="shared" si="13"/>
         <v>7</v>
       </c>
-      <c r="V86" s="15" t="e">
+      <c r="V86" s="15">
         <f>DATEDIF(Summary!$B$7,R86,"d")+1</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="W86" s="15">
+        <v>8</v>
+      </c>
+      <c r="W86" s="15" t="e">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="X86">
         <v>154</v>
@@ -12592,66 +12626,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="41"/>
-      <c r="K2" s="76" t="s">
+      <c r="K2" s="77" t="s">
         <v>151</v>
       </c>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
-      <c r="N2" s="77"/>
-      <c r="O2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="79"/>
       <c r="P2" s="42"/>
-      <c r="Q2" s="76" t="s">
+      <c r="Q2" s="77" t="s">
         <v>152</v>
       </c>
-      <c r="R2" s="79"/>
-      <c r="S2" s="79"/>
-      <c r="T2" s="78"/>
+      <c r="R2" s="80"/>
+      <c r="S2" s="80"/>
+      <c r="T2" s="79"/>
       <c r="U2" s="43"/>
-      <c r="V2" s="68" t="s">
+      <c r="V2" s="69" t="s">
         <v>153</v>
       </c>
-      <c r="W2" s="69"/>
-      <c r="X2" s="69"/>
-      <c r="Y2" s="70"/>
+      <c r="W2" s="70"/>
+      <c r="X2" s="70"/>
+      <c r="Y2" s="71"/>
       <c r="Z2" s="44"/>
-      <c r="AA2" s="68" t="s">
+      <c r="AA2" s="69" t="s">
         <v>154</v>
       </c>
-      <c r="AB2" s="69"/>
-      <c r="AC2" s="69"/>
-      <c r="AD2" s="69"/>
-      <c r="AE2" s="69"/>
-      <c r="AF2" s="69"/>
-      <c r="AG2" s="70"/>
+      <c r="AB2" s="70"/>
+      <c r="AC2" s="70"/>
+      <c r="AD2" s="70"/>
+      <c r="AE2" s="70"/>
+      <c r="AF2" s="70"/>
+      <c r="AG2" s="71"/>
       <c r="AH2" s="45"/>
-      <c r="AI2" s="68" t="s">
+      <c r="AI2" s="69" t="s">
         <v>155</v>
       </c>
-      <c r="AJ2" s="69"/>
-      <c r="AK2" s="69"/>
-      <c r="AL2" s="69"/>
-      <c r="AM2" s="69"/>
-      <c r="AN2" s="69"/>
-      <c r="AO2" s="69"/>
-      <c r="AP2" s="69"/>
+      <c r="AJ2" s="70"/>
+      <c r="AK2" s="70"/>
+      <c r="AL2" s="70"/>
+      <c r="AM2" s="70"/>
+      <c r="AN2" s="70"/>
+      <c r="AO2" s="70"/>
+      <c r="AP2" s="70"/>
     </row>
     <row r="3" spans="2:462" s="55" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="72" t="s">
         <v>156</v>
       </c>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="74" t="s">
         <v>157</v>
       </c>
-      <c r="D3" s="73" t="s">
+      <c r="D3" s="74" t="s">
         <v>158</v>
       </c>
-      <c r="E3" s="73" t="s">
+      <c r="E3" s="74" t="s">
         <v>159</v>
       </c>
-      <c r="F3" s="73" t="s">
+      <c r="F3" s="74" t="s">
         <v>160</v>
       </c>
-      <c r="G3" s="75" t="s">
+      <c r="G3" s="76" t="s">
         <v>161</v>
       </c>
       <c r="H3" s="57" t="s">
@@ -12678,12 +12712,12 @@
       <c r="AA3" s="56"/>
     </row>
     <row r="4" spans="2:462" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="72"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
       <c r="H4" s="47">
         <v>1</v>
       </c>
@@ -14063,9 +14097,9 @@
         <f>Tasks!V8</f>
         <v>1</v>
       </c>
-      <c r="F9" s="54" t="e">
+      <c r="F9" s="54">
         <f>Tasks!W8</f>
-        <v>#NUM!</v>
+        <v>2</v>
       </c>
       <c r="G9" s="49">
         <f>Tasks!Z8</f>
@@ -14089,9 +14123,9 @@
         <f>Tasks!V9</f>
         <v>1</v>
       </c>
-      <c r="F10" s="54" t="e">
+      <c r="F10" s="54">
         <f>Tasks!W9</f>
-        <v>#NUM!</v>
+        <v>7</v>
       </c>
       <c r="G10" s="49">
         <f>Tasks!Z9</f>
@@ -14115,9 +14149,9 @@
         <f>Tasks!V10</f>
         <v>1</v>
       </c>
-      <c r="F11" s="54" t="e">
+      <c r="F11" s="54">
         <f>Tasks!W10</f>
-        <v>#NUM!</v>
+        <v>7</v>
       </c>
       <c r="G11" s="49">
         <f>Tasks!Z10</f>
@@ -14141,9 +14175,9 @@
         <f>Tasks!V11</f>
         <v>1</v>
       </c>
-      <c r="F12" s="54" t="e">
+      <c r="F12" s="54">
         <f>Tasks!W11</f>
-        <v>#NUM!</v>
+        <v>7</v>
       </c>
       <c r="G12" s="49">
         <f>Tasks!Z11</f>
@@ -15753,9 +15787,9 @@
         <f>Tasks!V73</f>
         <v>1</v>
       </c>
-      <c r="F74" s="54" t="e">
+      <c r="F74" s="54">
         <f>Tasks!W73</f>
-        <v>#NUM!</v>
+        <v>7</v>
       </c>
       <c r="G74" s="49">
         <f>Tasks!Z73</f>
@@ -15779,9 +15813,9 @@
         <f>Tasks!V74</f>
         <v>1</v>
       </c>
-      <c r="F75" s="54" t="e">
+      <c r="F75" s="54">
         <f>Tasks!W74</f>
-        <v>#NUM!</v>
+        <v>7</v>
       </c>
       <c r="G75" s="49">
         <f>Tasks!Z74</f>
@@ -15805,9 +15839,9 @@
         <f>Tasks!V75</f>
         <v>1</v>
       </c>
-      <c r="F76" s="54" t="e">
+      <c r="F76" s="54">
         <f>Tasks!W75</f>
-        <v>#NUM!</v>
+        <v>7</v>
       </c>
       <c r="G76" s="49">
         <f>Tasks!Z75</f>
@@ -15831,9 +15865,9 @@
         <f>Tasks!V76</f>
         <v>1</v>
       </c>
-      <c r="F77" s="54" t="e">
+      <c r="F77" s="54">
         <f>Tasks!W76</f>
-        <v>#NUM!</v>
+        <v>7</v>
       </c>
       <c r="G77" s="49">
         <f>Tasks!Z76</f>
@@ -15857,9 +15891,9 @@
         <f>Tasks!V77</f>
         <v>1</v>
       </c>
-      <c r="F78" s="54" t="e">
+      <c r="F78" s="54">
         <f>Tasks!W77</f>
-        <v>#NUM!</v>
+        <v>7</v>
       </c>
       <c r="G78" s="49">
         <f>Tasks!Z77</f>
@@ -15883,9 +15917,9 @@
         <f>Tasks!V78</f>
         <v>1</v>
       </c>
-      <c r="F79" s="54" t="e">
+      <c r="F79" s="54">
         <f>Tasks!W78</f>
-        <v>#NUM!</v>
+        <v>7</v>
       </c>
       <c r="G79" s="49">
         <f>Tasks!Z78</f>
@@ -15909,9 +15943,9 @@
         <f>Tasks!V79</f>
         <v>1</v>
       </c>
-      <c r="F80" s="54" t="e">
+      <c r="F80" s="54">
         <f>Tasks!W79</f>
-        <v>#NUM!</v>
+        <v>7</v>
       </c>
       <c r="G80" s="49">
         <f>Tasks!Z79</f>
@@ -15935,9 +15969,9 @@
         <f>Tasks!V80</f>
         <v>1</v>
       </c>
-      <c r="F81" s="54" t="e">
+      <c r="F81" s="54">
         <f>Tasks!W80</f>
-        <v>#NUM!</v>
+        <v>7</v>
       </c>
       <c r="G81" s="49">
         <f>Tasks!Z80</f>
@@ -15961,9 +15995,9 @@
         <f>Tasks!V81</f>
         <v>1</v>
       </c>
-      <c r="F82" s="54" t="e">
+      <c r="F82" s="54">
         <f>Tasks!W81</f>
-        <v>#NUM!</v>
+        <v>7</v>
       </c>
       <c r="G82" s="49">
         <f>Tasks!Z81</f>
@@ -16009,13 +16043,13 @@
         <f>Tasks!U83</f>
         <v>7</v>
       </c>
-      <c r="E84" s="54" t="e">
+      <c r="E84" s="54">
         <f>Tasks!V83</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F84" s="54">
+        <v>8</v>
+      </c>
+      <c r="F84" s="54" t="e">
         <f>Tasks!W83</f>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="G84" s="49">
         <f>Tasks!Z83</f>
@@ -16035,13 +16069,13 @@
         <f>Tasks!U84</f>
         <v>7</v>
       </c>
-      <c r="E85" s="54" t="e">
+      <c r="E85" s="54">
         <f>Tasks!V84</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F85" s="54">
+        <v>8</v>
+      </c>
+      <c r="F85" s="54" t="e">
         <f>Tasks!W84</f>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="G85" s="49">
         <f>Tasks!Z84</f>
@@ -16061,13 +16095,13 @@
         <f>Tasks!U85</f>
         <v>7</v>
       </c>
-      <c r="E86" s="54" t="e">
+      <c r="E86" s="54">
         <f>Tasks!V85</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F86" s="54">
+        <v>8</v>
+      </c>
+      <c r="F86" s="54" t="e">
         <f>Tasks!W85</f>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="G86" s="49">
         <f>Tasks!Z85</f>
@@ -16087,13 +16121,13 @@
         <f>Tasks!U86</f>
         <v>7</v>
       </c>
-      <c r="E87" s="54" t="e">
+      <c r="E87" s="54">
         <f>Tasks!V86</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F87" s="54">
+        <v>8</v>
+      </c>
+      <c r="F87" s="54" t="e">
         <f>Tasks!W86</f>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="G87" s="49">
         <f>Tasks!Z86</f>
@@ -18316,7 +18350,7 @@
   <dimension ref="A2:H26"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18451,22 +18485,22 @@
         <v>3</v>
       </c>
       <c r="C13" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
@@ -18477,22 +18511,22 @@
         <v>4</v>
       </c>
       <c r="C14" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -18509,16 +18543,16 @@
         <v>0</v>
       </c>
       <c r="E15" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -18529,22 +18563,22 @@
         <v>6</v>
       </c>
       <c r="C16" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -18554,12 +18588,24 @@
       <c r="B17">
         <v>7</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
+      <c r="C17" s="12">
+        <v>1</v>
+      </c>
+      <c r="D17" s="12">
+        <v>1</v>
+      </c>
+      <c r="E17" s="12">
+        <v>1</v>
+      </c>
+      <c r="F17" s="12">
+        <v>1</v>
+      </c>
+      <c r="G17" s="12">
+        <v>1</v>
+      </c>
+      <c r="H17" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
@@ -18640,27 +18686,27 @@
       </c>
       <c r="C26">
         <f t="shared" ref="C26:H26" si="0">SUM(C11:C23)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E26">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G26">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H26">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -19244,7 +19290,7 @@
       </c>
       <c r="B33">
         <f>Summary!$B$39-Attendance!C26</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L33" s="13"/>
     </row>
@@ -19254,7 +19300,7 @@
       </c>
       <c r="B34">
         <f>Summary!$B$39-Attendance!D26</f>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="L34" s="13"/>
     </row>
@@ -19264,7 +19310,7 @@
       </c>
       <c r="B35">
         <f>Summary!$B$39-Attendance!E26</f>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="L35" s="13"/>
     </row>
@@ -19274,7 +19320,7 @@
       </c>
       <c r="B36">
         <f>Summary!$B$39-Attendance!F26</f>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="L36" s="13"/>
     </row>
@@ -19284,7 +19330,7 @@
       </c>
       <c r="B37">
         <f>Summary!$B$39-Attendance!G26</f>
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
@@ -19293,7 +19339,7 @@
       </c>
       <c r="B38">
         <f>Summary!$B$39-Attendance!H26</f>
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.35">
@@ -19307,7 +19353,7 @@
       </c>
       <c r="B41">
         <f>-1*B33*Summary!$B$40</f>
-        <v>-81.818181818181827</v>
+        <v>-45.45454545454546</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.35">
@@ -19316,7 +19362,7 @@
       </c>
       <c r="B42">
         <f>-1*B34*Summary!$B$40</f>
-        <v>-90.909090909090921</v>
+        <v>-54.545454545454547</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.35">
@@ -19325,7 +19371,7 @@
       </c>
       <c r="B43">
         <f>-1*B35*Summary!$B$40</f>
-        <v>-81.818181818181827</v>
+        <v>-36.363636363636367</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.35">
@@ -19334,7 +19380,7 @@
       </c>
       <c r="B44">
         <f>-1*B36*Summary!$B$40</f>
-        <v>-81.818181818181827</v>
+        <v>-36.363636363636367</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.35">
@@ -19343,7 +19389,7 @@
       </c>
       <c r="B45">
         <f>-1*B37*Summary!$B$40</f>
-        <v>-81.818181818181827</v>
+        <v>-36.363636363636367</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.35">
@@ -19352,7 +19398,7 @@
       </c>
       <c r="B46">
         <f>-1*B38*Summary!$B$40</f>
-        <v>-81.818181818181827</v>
+        <v>-36.363636363636367</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.35">
@@ -19921,6 +19967,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="19dc0929-3265-432c-90cd-a4a18b147cbc" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100425D870C9FE3FA459BE7BAB817912A28" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2888a6b5c62326ad14675b6ae20d83ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="19dc0929-3265-432c-90cd-a4a18b147cbc" xmlns:ns4="e15c2e9d-9071-420f-8402-443b554f1232" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="df22a33983a74acd15e217796b17182e" ns3:_="" ns4:_="">
     <xsd:import namespace="19dc0929-3265-432c-90cd-a4a18b147cbc"/>
@@ -20167,24 +20230,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A377B27C-73B5-421A-9BAA-7FB75238CE4F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="e15c2e9d-9071-420f-8402-443b554f1232"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="19dc0929-3265-432c-90cd-a4a18b147cbc"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="19dc0929-3265-432c-90cd-a4a18b147cbc" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75E4E88A-17F8-40B2-8EC1-AE408CF7AA54}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F9BD7DA-52C8-49CE-B9E2-21F98F087543}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20201,29 +20272,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75E4E88A-17F8-40B2-8EC1-AE408CF7AA54}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A377B27C-73B5-421A-9BAA-7FB75238CE4F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="e15c2e9d-9071-420f-8402-443b554f1232"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="19dc0929-3265-432c-90cd-a4a18b147cbc"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update top_level_task_sheet_schedule_decoupled-V1.xlsx with revised data and formatting
</commit_message>
<xml_diff>
--- a/artifacts/top_level_task_sheet_schedule_decoupled-V1.xlsx
+++ b/artifacts/top_level_task_sheet_schedule_decoupled-V1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\spring-2025\Compilers\LABs\lab-schedule-decoupled\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A159AF1-0A1A-463E-95C4-9DE99F97BAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83735342-B7D2-4AAD-B3E8-625ED5C87145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -2851,7 +2851,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1FC06A3-543F-4971-A317-96FE7AF52EC7}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -3195,27 +3195,27 @@
       </c>
       <c r="B26" s="23">
         <f>Attendance!C26</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C26" s="23">
         <f>Attendance!D26</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D26" s="23">
         <f>Attendance!E26</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E26" s="23">
         <f>Attendance!F26</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F26" s="23">
         <f>Attendance!G26</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G26" s="23">
         <f>Attendance!H26</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
@@ -3247,27 +3247,27 @@
       </c>
       <c r="B28" s="23">
         <f t="shared" ref="B28:G28" si="0">SUM(B26:B27)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C28" s="23">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D28" s="23">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E28" s="23">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F28" s="23">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G28" s="23">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
@@ -3276,7 +3276,7 @@
       </c>
       <c r="B30" s="23">
         <f>SUM(B28:G28)</f>
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
@@ -3463,7 +3463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D498C59D-E060-40B6-B59A-036A9DD1C81C}">
   <dimension ref="A1:AC152"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A66" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="Q87" sqref="Q87"/>
     </sheetView>
   </sheetViews>
@@ -18350,7 +18350,7 @@
   <dimension ref="A2:H26"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18614,12 +18614,24 @@
       <c r="B18">
         <v>8</v>
       </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
+      <c r="C18" s="12">
+        <v>1</v>
+      </c>
+      <c r="D18" s="12">
+        <v>1</v>
+      </c>
+      <c r="E18" s="12">
+        <v>1</v>
+      </c>
+      <c r="F18" s="12">
+        <v>1</v>
+      </c>
+      <c r="G18" s="12">
+        <v>1</v>
+      </c>
+      <c r="H18" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
@@ -18686,27 +18698,27 @@
       </c>
       <c r="C26">
         <f t="shared" ref="C26:H26" si="0">SUM(C11:C23)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E26">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G26">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H26">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -19086,7 +19098,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{861C5F3C-2BB8-48C2-B1E4-E1F141881B60}">
   <dimension ref="A1:Q81"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
@@ -19290,7 +19302,7 @@
       </c>
       <c r="B33">
         <f>Summary!$B$39-Attendance!C26</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L33" s="13"/>
     </row>
@@ -19300,7 +19312,7 @@
       </c>
       <c r="B34">
         <f>Summary!$B$39-Attendance!D26</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L34" s="13"/>
     </row>
@@ -19310,7 +19322,7 @@
       </c>
       <c r="B35">
         <f>Summary!$B$39-Attendance!E26</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L35" s="13"/>
     </row>
@@ -19320,7 +19332,7 @@
       </c>
       <c r="B36">
         <f>Summary!$B$39-Attendance!F26</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L36" s="13"/>
     </row>
@@ -19330,7 +19342,7 @@
       </c>
       <c r="B37">
         <f>Summary!$B$39-Attendance!G26</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
@@ -19339,7 +19351,7 @@
       </c>
       <c r="B38">
         <f>Summary!$B$39-Attendance!H26</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.35">
@@ -19353,7 +19365,7 @@
       </c>
       <c r="B41">
         <f>-1*B33*Summary!$B$40</f>
-        <v>-45.45454545454546</v>
+        <v>-36.363636363636367</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.35">
@@ -19362,7 +19374,7 @@
       </c>
       <c r="B42">
         <f>-1*B34*Summary!$B$40</f>
-        <v>-54.545454545454547</v>
+        <v>-45.45454545454546</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.35">
@@ -19371,7 +19383,7 @@
       </c>
       <c r="B43">
         <f>-1*B35*Summary!$B$40</f>
-        <v>-36.363636363636367</v>
+        <v>-27.272727272727273</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.35">
@@ -19380,7 +19392,7 @@
       </c>
       <c r="B44">
         <f>-1*B36*Summary!$B$40</f>
-        <v>-36.363636363636367</v>
+        <v>-27.272727272727273</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.35">
@@ -19389,7 +19401,7 @@
       </c>
       <c r="B45">
         <f>-1*B37*Summary!$B$40</f>
-        <v>-36.363636363636367</v>
+        <v>-27.272727272727273</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.35">
@@ -19398,7 +19410,7 @@
       </c>
       <c r="B46">
         <f>-1*B38*Summary!$B$40</f>
-        <v>-36.363636363636367</v>
+        <v>-27.272727272727273</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.35">
@@ -19967,23 +19979,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="19dc0929-3265-432c-90cd-a4a18b147cbc" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100425D870C9FE3FA459BE7BAB817912A28" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2888a6b5c62326ad14675b6ae20d83ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="19dc0929-3265-432c-90cd-a4a18b147cbc" xmlns:ns4="e15c2e9d-9071-420f-8402-443b554f1232" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="df22a33983a74acd15e217796b17182e" ns3:_="" ns4:_="">
     <xsd:import namespace="19dc0929-3265-432c-90cd-a4a18b147cbc"/>
@@ -20230,32 +20225,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A377B27C-73B5-421A-9BAA-7FB75238CE4F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="e15c2e9d-9071-420f-8402-443b554f1232"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="19dc0929-3265-432c-90cd-a4a18b147cbc"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75E4E88A-17F8-40B2-8EC1-AE408CF7AA54}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="19dc0929-3265-432c-90cd-a4a18b147cbc" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F9BD7DA-52C8-49CE-B9E2-21F98F087543}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20272,4 +20259,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75E4E88A-17F8-40B2-8EC1-AE408CF7AA54}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A377B27C-73B5-421A-9BAA-7FB75238CE4F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="e15c2e9d-9071-420f-8402-443b554f1232"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="19dc0929-3265-432c-90cd-a4a18b147cbc"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add new Excel files for top-level task sheet schedule
- Introduced a new binary file: top_level_task_sheet_schedule_decoupled-V1 (version 1).xlsb.xlsx
- Updated existing binary file: top_level_task_sheet_schedule_decoupled-V1.xlsx
</commit_message>
<xml_diff>
--- a/artifacts/top_level_task_sheet_schedule_decoupled-V1.xlsx
+++ b/artifacts/top_level_task_sheet_schedule_decoupled-V1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\spring-2025\Compilers\LABs\lab-schedule-decoupled\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83735342-B7D2-4AAD-B3E8-625ED5C87145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B0C05A-4222-484F-9CA8-7EDDF7C9C2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="386">
   <si>
     <t>Task</t>
   </si>
@@ -1790,6 +1790,12 @@
   </si>
   <si>
     <t>garrett.w.snow-1@ou.edu</t>
+  </si>
+  <si>
+    <t>madylin.d.teel-1@ou.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Madylin Teel </t>
   </si>
 </sst>
 </file>
@@ -2994,8 +3000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DE25F09-78F6-4E9B-82D7-25CE88A172A9}">
   <dimension ref="A2:G48"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3081,8 +3087,12 @@
       <c r="A12" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
+      <c r="B12" s="16" t="s">
+        <v>385</v>
+      </c>
+      <c r="C12" s="67" t="s">
+        <v>384</v>
+      </c>
       <c r="D12" s="16"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -3195,27 +3205,27 @@
       </c>
       <c r="B26" s="23">
         <f>Attendance!C26</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C26" s="23">
         <f>Attendance!D26</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D26" s="23">
         <f>Attendance!E26</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E26" s="23">
         <f>Attendance!F26</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F26" s="23">
         <f>Attendance!G26</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G26" s="23">
         <f>Attendance!H26</f>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
@@ -3247,27 +3257,27 @@
       </c>
       <c r="B28" s="23">
         <f t="shared" ref="B28:G28" si="0">SUM(B26:B27)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C28" s="23">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D28" s="23">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E28" s="23">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F28" s="23">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G28" s="23">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
@@ -3276,7 +3286,7 @@
       </c>
       <c r="B30" s="23">
         <f>SUM(B28:G28)</f>
-        <v>45</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
@@ -3293,7 +3303,7 @@
       </c>
       <c r="B33" s="23">
         <f>Tasks!B151</f>
-        <v>20</v>
+        <v>875</v>
       </c>
       <c r="C33" s="23">
         <f>Tasks!AC141</f>
@@ -3332,7 +3342,7 @@
         <v>49</v>
       </c>
       <c r="B39" s="25">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D39" t="s">
         <v>372</v>
@@ -3344,7 +3354,7 @@
       </c>
       <c r="B40" s="25">
         <f>100/B39</f>
-        <v>9.0909090909090917</v>
+        <v>8.3333333333333339</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
@@ -3410,20 +3420,19 @@
         <v>107</v>
       </c>
       <c r="B47" s="25">
-        <f>B37/4</f>
-        <v>303.75</v>
+        <v>243</v>
       </c>
       <c r="C47" s="25">
         <f>B47*0.9</f>
-        <v>273.375</v>
+        <v>218.70000000000002</v>
       </c>
       <c r="D47" s="25">
         <f>B47*0.8</f>
-        <v>243</v>
+        <v>194.4</v>
       </c>
       <c r="E47" s="25">
         <f>B47*0.7</f>
-        <v>212.625</v>
+        <v>170.1</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
@@ -3431,20 +3440,19 @@
         <v>108</v>
       </c>
       <c r="B48" s="25">
-        <f>B38/4</f>
-        <v>364.5</v>
+        <v>243</v>
       </c>
       <c r="C48" s="25">
         <f>B48*0.9</f>
-        <v>328.05</v>
+        <v>218.70000000000002</v>
       </c>
       <c r="D48" s="25">
         <f>B48*0.8</f>
-        <v>291.60000000000002</v>
+        <v>194.4</v>
       </c>
       <c r="E48" s="25">
         <f>B48*0.7</f>
-        <v>255.14999999999998</v>
+        <v>170.1</v>
       </c>
     </row>
   </sheetData>
@@ -3454,6 +3462,7 @@
     <hyperlink ref="C14" r:id="rId3" xr:uid="{848825A5-8BA1-4266-853B-28B51E51C25D}"/>
     <hyperlink ref="C15" r:id="rId4" xr:uid="{9A9C7C4C-01EC-4A42-9106-087D5D248881}"/>
     <hyperlink ref="C16" r:id="rId5" xr:uid="{B5996B87-A084-453E-B665-30E5008459C2}"/>
+    <hyperlink ref="C12" r:id="rId6" xr:uid="{E73D67DE-6F42-4BF7-BA35-6C8F60BAD3F1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3463,8 +3472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D498C59D-E060-40B6-B59A-036A9DD1C81C}">
   <dimension ref="A1:AC152"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q87" sqref="Q87"/>
+    <sheetView topLeftCell="A115" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4279,11 +4288,11 @@
       </c>
       <c r="Y12" s="16"/>
       <c r="Z12" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA12" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB12" s="14">
         <v>0</v>
@@ -4349,11 +4358,11 @@
       </c>
       <c r="Y13" s="16"/>
       <c r="Z13" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA13" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB13" s="14">
         <v>0</v>
@@ -4547,11 +4556,11 @@
       </c>
       <c r="Y16" s="16"/>
       <c r="Z16" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA16" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB16" s="14">
         <v>0</v>
@@ -4613,11 +4622,11 @@
       </c>
       <c r="Y17" s="16"/>
       <c r="Z17" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA17" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB17" s="14">
         <v>0</v>
@@ -4681,11 +4690,11 @@
       </c>
       <c r="Y18" s="16"/>
       <c r="Z18" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA18" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB18" s="14">
         <v>0</v>
@@ -4749,11 +4758,11 @@
       </c>
       <c r="Y19" s="16"/>
       <c r="Z19" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA19" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB19" s="14">
         <v>0</v>
@@ -4817,11 +4826,11 @@
       </c>
       <c r="Y20" s="16"/>
       <c r="Z20" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA20" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB20" s="14">
         <v>0</v>
@@ -4885,11 +4894,11 @@
       </c>
       <c r="Y21" s="16"/>
       <c r="Z21" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA21" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB21" s="14">
         <v>0</v>
@@ -4955,11 +4964,11 @@
       </c>
       <c r="Y22" s="16"/>
       <c r="Z22" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA22" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB22" s="14">
         <v>0</v>
@@ -5023,11 +5032,11 @@
       </c>
       <c r="Y23" s="16"/>
       <c r="Z23" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA23" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB23" s="14">
         <v>0</v>
@@ -5256,11 +5265,11 @@
       </c>
       <c r="Y27" s="16"/>
       <c r="Z27" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA27" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB27" s="14">
         <v>0</v>
@@ -5322,11 +5331,11 @@
       </c>
       <c r="Y28" s="16"/>
       <c r="Z28" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA28" s="15">
         <f t="shared" ref="AA28:AA58" si="6">(B28+C28)*Z28</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB28" s="14">
         <v>0</v>
@@ -5388,11 +5397,11 @@
       </c>
       <c r="Y29" s="16"/>
       <c r="Z29" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA29" s="15">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB29" s="14">
         <v>0</v>
@@ -5454,11 +5463,11 @@
       </c>
       <c r="Y30" s="16"/>
       <c r="Z30" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA30" s="15">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB30" s="14">
         <v>0</v>
@@ -5687,11 +5696,11 @@
       </c>
       <c r="Y34" s="16"/>
       <c r="Z34" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA34" s="15">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AB34" s="14">
         <v>0</v>
@@ -5750,11 +5759,11 @@
       </c>
       <c r="Y35" s="16"/>
       <c r="Z35" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA35" s="15">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AB35" s="14">
         <v>0</v>
@@ -5813,11 +5822,11 @@
       </c>
       <c r="Y36" s="16"/>
       <c r="Z36" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA36" s="15">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AB36" s="14">
         <v>0</v>
@@ -5935,11 +5944,11 @@
       </c>
       <c r="Y38" s="16"/>
       <c r="Z38" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA38" s="15">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AB38" s="14">
         <v>0</v>
@@ -5998,11 +6007,11 @@
       </c>
       <c r="Y39" s="16"/>
       <c r="Z39" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA39" s="15">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AB39" s="14">
         <v>0</v>
@@ -6061,11 +6070,11 @@
       </c>
       <c r="Y40" s="16"/>
       <c r="Z40" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA40" s="15">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AB40" s="14">
         <v>0</v>
@@ -6124,11 +6133,11 @@
       </c>
       <c r="Y41" s="16"/>
       <c r="Z41" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA41" s="15">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AB41" s="14">
         <v>0</v>
@@ -6190,11 +6199,11 @@
       </c>
       <c r="Y42" s="16"/>
       <c r="Z42" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA42" s="15">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AB42" s="14">
         <v>0</v>
@@ -6312,11 +6321,11 @@
       </c>
       <c r="Y44" s="16"/>
       <c r="Z44" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA44" s="15">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB44" s="14">
         <v>0</v>
@@ -6378,11 +6387,11 @@
       </c>
       <c r="Y45" s="16"/>
       <c r="Z45" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA45" s="15">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB45" s="14">
         <v>0</v>
@@ -6444,11 +6453,11 @@
       </c>
       <c r="Y46" s="16"/>
       <c r="Z46" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA46" s="15">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB46" s="14">
         <v>0</v>
@@ -6510,11 +6519,11 @@
       </c>
       <c r="Y47" s="16"/>
       <c r="Z47" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA47" s="15">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB47" s="14">
         <v>0</v>
@@ -6632,11 +6641,11 @@
       </c>
       <c r="Y49" s="16"/>
       <c r="Z49" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA49" s="15">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB49" s="14">
         <v>0</v>
@@ -6698,11 +6707,11 @@
       </c>
       <c r="Y50" s="16"/>
       <c r="Z50" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA50" s="15">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AB50" s="14">
         <v>0</v>
@@ -8170,11 +8179,11 @@
       </c>
       <c r="Y73" s="16"/>
       <c r="Z73" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA73" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB73" s="14">
         <v>0</v>
@@ -8240,11 +8249,11 @@
       </c>
       <c r="Y74" s="16"/>
       <c r="Z74" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA74" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB74" s="14">
         <v>0</v>
@@ -8310,11 +8319,11 @@
       </c>
       <c r="Y75" s="16"/>
       <c r="Z75" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA75" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB75" s="14">
         <v>0</v>
@@ -8357,7 +8366,7 @@
         <v>45720</v>
       </c>
       <c r="S76" s="61">
-        <v>45727</v>
+        <v>45741</v>
       </c>
       <c r="T76" s="15">
         <f>DATEDIF(Summary!$B$7,P76,"d")+1</f>
@@ -8373,18 +8382,18 @@
       </c>
       <c r="W76" s="15">
         <f t="shared" si="14"/>
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="X76">
         <v>144</v>
       </c>
       <c r="Y76" s="16"/>
       <c r="Z76" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA76" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB76" s="14">
         <v>0</v>
@@ -8427,7 +8436,7 @@
         <v>45720</v>
       </c>
       <c r="S77" s="61">
-        <v>45727</v>
+        <v>45741</v>
       </c>
       <c r="T77" s="15">
         <f>DATEDIF(Summary!$B$7,P77,"d")+1</f>
@@ -8443,18 +8452,18 @@
       </c>
       <c r="W77" s="15">
         <f t="shared" si="14"/>
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="X77">
         <v>145</v>
       </c>
       <c r="Y77" s="16"/>
       <c r="Z77" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA77" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB77" s="14">
         <v>0</v>
@@ -8520,11 +8529,11 @@
       </c>
       <c r="Y78" s="16"/>
       <c r="Z78" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA78" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB78" s="14">
         <v>0</v>
@@ -8590,11 +8599,11 @@
       </c>
       <c r="Y79" s="16"/>
       <c r="Z79" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA79" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB79" s="14">
         <v>0</v>
@@ -8660,11 +8669,11 @@
       </c>
       <c r="Y80" s="16"/>
       <c r="Z80" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA80" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB80" s="14">
         <v>0</v>
@@ -8730,11 +8739,11 @@
       </c>
       <c r="Y81" s="16"/>
       <c r="Z81" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA81" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB81" s="14">
         <v>0</v>
@@ -8922,11 +8931,11 @@
       </c>
       <c r="Y84" s="16"/>
       <c r="Z84" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA84" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB84" s="14">
         <v>0</v>
@@ -8966,9 +8975,11 @@
         <v>45734</v>
       </c>
       <c r="R85" s="61">
-        <v>45727</v>
-      </c>
-      <c r="S85" s="61"/>
+        <v>45741</v>
+      </c>
+      <c r="S85" s="61">
+        <v>45743</v>
+      </c>
       <c r="T85" s="15">
         <f>DATEDIF(Summary!$B$7,P85,"d")+1</f>
         <v>8</v>
@@ -8979,22 +8990,22 @@
       </c>
       <c r="V85" s="15">
         <f>DATEDIF(Summary!$B$7,R85,"d")+1</f>
-        <v>8</v>
-      </c>
-      <c r="W85" s="15" t="e">
+        <v>22</v>
+      </c>
+      <c r="W85" s="15">
         <f t="shared" si="14"/>
-        <v>#NUM!</v>
+        <v>2</v>
       </c>
       <c r="X85">
         <v>153</v>
       </c>
       <c r="Y85" s="16"/>
       <c r="Z85" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA85" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB85" s="14">
         <v>0</v>
@@ -9058,11 +9069,11 @@
       </c>
       <c r="Y86" s="16"/>
       <c r="Z86" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA86" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB86" s="14">
         <v>0</v>
@@ -9180,11 +9191,11 @@
       </c>
       <c r="Y88" s="16"/>
       <c r="Z88" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA88" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB88" s="14">
         <v>0</v>
@@ -9246,11 +9257,11 @@
       </c>
       <c r="Y89" s="16"/>
       <c r="Z89" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA89" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB89" s="14">
         <v>0</v>
@@ -9312,11 +9323,11 @@
       </c>
       <c r="Y90" s="16"/>
       <c r="Z90" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA90" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB90" s="14">
         <v>0</v>
@@ -9378,11 +9389,11 @@
       </c>
       <c r="Y91" s="16"/>
       <c r="Z91" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA91" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB91" s="14">
         <v>0</v>
@@ -9444,11 +9455,11 @@
       </c>
       <c r="Y92" s="16"/>
       <c r="Z92" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA92" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB92" s="14">
         <v>0</v>
@@ -9487,8 +9498,12 @@
         <f t="shared" si="17"/>
         <v>45741</v>
       </c>
-      <c r="R93" s="61"/>
-      <c r="S93" s="61"/>
+      <c r="R93" s="61">
+        <v>45743</v>
+      </c>
+      <c r="S93" s="61">
+        <v>45750</v>
+      </c>
       <c r="T93" s="15">
         <f>DATEDIF(Summary!$B$7,P93,"d")+1</f>
         <v>15</v>
@@ -9497,24 +9512,24 @@
         <f t="shared" si="13"/>
         <v>7</v>
       </c>
-      <c r="V93" s="15" t="e">
+      <c r="V93" s="15">
         <f>DATEDIF(Summary!$B$7,R93,"d")+1</f>
-        <v>#NUM!</v>
+        <v>24</v>
       </c>
       <c r="W93" s="15">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="X93">
         <v>161</v>
       </c>
       <c r="Y93" s="16"/>
       <c r="Z93" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA93" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB93" s="14">
         <v>0</v>
@@ -9576,11 +9591,11 @@
       </c>
       <c r="Y94" s="16"/>
       <c r="Z94" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA94" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB94" s="14">
         <v>0</v>
@@ -9619,8 +9634,12 @@
         <f t="shared" si="17"/>
         <v>45741</v>
       </c>
-      <c r="R95" s="61"/>
-      <c r="S95" s="61"/>
+      <c r="R95" s="61">
+        <v>45755</v>
+      </c>
+      <c r="S95" s="61">
+        <v>45755</v>
+      </c>
       <c r="T95" s="15">
         <f>DATEDIF(Summary!$B$7,P95,"d")+1</f>
         <v>15</v>
@@ -9629,9 +9648,9 @@
         <f t="shared" si="13"/>
         <v>7</v>
       </c>
-      <c r="V95" s="15" t="e">
+      <c r="V95" s="15">
         <f>DATEDIF(Summary!$B$7,R95,"d")+1</f>
-        <v>#NUM!</v>
+        <v>36</v>
       </c>
       <c r="W95" s="15">
         <f t="shared" si="14"/>
@@ -9642,11 +9661,11 @@
       </c>
       <c r="Y95" s="16"/>
       <c r="Z95" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA95" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB95" s="14">
         <v>0</v>
@@ -9708,11 +9727,11 @@
       </c>
       <c r="Y96" s="16"/>
       <c r="Z96" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA96" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB96" s="14">
         <v>0</v>
@@ -9939,8 +9958,12 @@
         <f t="shared" si="20"/>
         <v>45748</v>
       </c>
-      <c r="R100" s="61"/>
-      <c r="S100" s="61"/>
+      <c r="R100" s="61">
+        <v>45755</v>
+      </c>
+      <c r="S100" s="61">
+        <v>45755</v>
+      </c>
       <c r="T100" s="15">
         <f>DATEDIF(Summary!$B$7,P100,"d")+1</f>
         <v>22</v>
@@ -9949,9 +9972,9 @@
         <f t="shared" si="13"/>
         <v>7</v>
       </c>
-      <c r="V100" s="15" t="e">
+      <c r="V100" s="15">
         <f>DATEDIF(Summary!$B$7,R100,"d")+1</f>
-        <v>#NUM!</v>
+        <v>36</v>
       </c>
       <c r="W100" s="15">
         <f t="shared" si="14"/>
@@ -9962,11 +9985,11 @@
       </c>
       <c r="Y100" s="16"/>
       <c r="Z100" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA100" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB100" s="14">
         <v>0</v>
@@ -10028,11 +10051,11 @@
       </c>
       <c r="Y101" s="16"/>
       <c r="Z101" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA101" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB101" s="14">
         <v>0</v>
@@ -10160,11 +10183,11 @@
       </c>
       <c r="Y103" s="16"/>
       <c r="Z103" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA103" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB103" s="14">
         <v>0</v>
@@ -10402,11 +10425,11 @@
       </c>
       <c r="Y107" s="16"/>
       <c r="Z107" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA107" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB107" s="14">
         <v>0</v>
@@ -10468,11 +10491,11 @@
       </c>
       <c r="Y108" s="16"/>
       <c r="Z108" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA108" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB108" s="14">
         <v>0</v>
@@ -10534,11 +10557,11 @@
       </c>
       <c r="Y109" s="16"/>
       <c r="Z109" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA109" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB109" s="14">
         <v>0</v>
@@ -10666,11 +10689,11 @@
       </c>
       <c r="Y111" s="16"/>
       <c r="Z111" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA111" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB111" s="14">
         <v>0</v>
@@ -10732,11 +10755,11 @@
       </c>
       <c r="Y112" s="16"/>
       <c r="Z112" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA112" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB112" s="14">
         <v>0</v>
@@ -10798,11 +10821,11 @@
       </c>
       <c r="Y113" s="16"/>
       <c r="Z113" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA113" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB113" s="14">
         <v>0</v>
@@ -10932,11 +10955,11 @@
       </c>
       <c r="Y115" s="16"/>
       <c r="Z115" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA115" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB115" s="14">
         <v>0</v>
@@ -10998,11 +11021,11 @@
       </c>
       <c r="Y116" s="16"/>
       <c r="Z116" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA116" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB116" s="14">
         <v>0</v>
@@ -11064,11 +11087,11 @@
       </c>
       <c r="Y117" s="16"/>
       <c r="Z117" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA117" s="15">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AB117" s="14">
         <v>0</v>
@@ -11463,14 +11486,14 @@
         <v>0</v>
       </c>
       <c r="AA123" s="15">
-        <f t="shared" ref="AA123:AA135" si="23">(B123+C123)*Z123</f>
+        <f t="shared" ref="AA123:AA141" si="23">(B123+C123)*Z123</f>
         <v>0</v>
       </c>
       <c r="AB123" s="14">
         <v>0</v>
       </c>
       <c r="AC123" s="23">
-        <f t="shared" ref="AC123:AC135" si="24">(B123+C123)*AB123</f>
+        <f t="shared" ref="AC123:AC141" si="24">(B123+C123)*AB123</f>
         <v>0</v>
       </c>
     </row>
@@ -11989,9 +12012,6 @@
         <v>224</v>
       </c>
       <c r="Y132" s="16"/>
-      <c r="Z132" s="16">
-        <v>0</v>
-      </c>
       <c r="AA132" s="15">
         <f t="shared" si="23"/>
         <v>0</v>
@@ -12056,11 +12076,11 @@
       </c>
       <c r="Y133" s="16"/>
       <c r="Z133" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA133" s="15">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AB133" s="14">
         <v>0</v>
@@ -12122,11 +12142,11 @@
       </c>
       <c r="Y134" s="16"/>
       <c r="Z134" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA134" s="15">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AB134" s="14">
         <v>0</v>
@@ -12188,11 +12208,11 @@
       </c>
       <c r="Y135" s="16"/>
       <c r="Z135" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA135" s="15">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AB135" s="14">
         <v>0</v>
@@ -12245,6 +12265,20 @@
       <c r="X136">
         <v>228</v>
       </c>
+      <c r="Z136" s="16">
+        <v>1</v>
+      </c>
+      <c r="AA136" s="15">
+        <f t="shared" si="23"/>
+        <v>20</v>
+      </c>
+      <c r="AB136" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC136" s="23">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="137" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A137" s="2"/>
@@ -12289,6 +12323,20 @@
       <c r="X137">
         <v>229</v>
       </c>
+      <c r="Z137" s="16">
+        <v>1</v>
+      </c>
+      <c r="AA137" s="15">
+        <f t="shared" si="23"/>
+        <v>20</v>
+      </c>
+      <c r="AB137" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC137" s="23">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="138" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A138" s="2"/>
@@ -12333,6 +12381,20 @@
       <c r="X138">
         <v>230</v>
       </c>
+      <c r="Z138" s="16">
+        <v>1</v>
+      </c>
+      <c r="AA138" s="15">
+        <f t="shared" si="23"/>
+        <v>20</v>
+      </c>
+      <c r="AB138" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC138" s="23">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="139" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A139" s="2"/>
@@ -12377,6 +12439,20 @@
       <c r="X139">
         <v>231</v>
       </c>
+      <c r="Z139" s="16">
+        <v>1</v>
+      </c>
+      <c r="AA139" s="15">
+        <f t="shared" si="23"/>
+        <v>20</v>
+      </c>
+      <c r="AB139" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC139" s="23">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="140" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A140" s="2"/>
@@ -12421,7 +12497,20 @@
       <c r="X140">
         <v>232</v>
       </c>
-      <c r="AC140" s="15"/>
+      <c r="Z140" s="16">
+        <v>1</v>
+      </c>
+      <c r="AA140" s="15">
+        <f t="shared" si="23"/>
+        <v>20</v>
+      </c>
+      <c r="AB140" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC140" s="23">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="141" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A141" s="2"/>
@@ -12466,7 +12555,20 @@
       <c r="X141">
         <v>233</v>
       </c>
-      <c r="AC141" s="21"/>
+      <c r="Z141" s="16">
+        <v>1</v>
+      </c>
+      <c r="AA141" s="15">
+        <f t="shared" si="23"/>
+        <v>5</v>
+      </c>
+      <c r="AB141" s="14">
+        <v>0</v>
+      </c>
+      <c r="AC141" s="23">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="142" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A142" s="2"/>
@@ -12556,7 +12658,7 @@
       </c>
       <c r="B151" s="15">
         <f>SUM(AA4:AA143)</f>
-        <v>20</v>
+        <v>875</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
@@ -12585,7 +12687,7 @@
   </sheetPr>
   <dimension ref="B1:QT169"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C22" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <selection activeCell="F3" sqref="F3:F4"/>
     </sheetView>
   </sheetViews>
@@ -14207,7 +14309,7 @@
       </c>
       <c r="G13" s="49">
         <f>Tasks!Z12</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:462" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -14233,7 +14335,7 @@
       </c>
       <c r="G14" s="49">
         <f>Tasks!Z13</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:462" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -14311,7 +14413,7 @@
       </c>
       <c r="G17" s="49">
         <f>Tasks!Z16</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -14337,7 +14439,7 @@
       </c>
       <c r="G18" s="49">
         <f>Tasks!Z17</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -14363,7 +14465,7 @@
       </c>
       <c r="G19" s="49">
         <f>Tasks!Z18</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -14389,7 +14491,7 @@
       </c>
       <c r="G20" s="49">
         <f>Tasks!Z19</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -14415,7 +14517,7 @@
       </c>
       <c r="G21" s="49">
         <f>Tasks!Z20</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -14441,7 +14543,7 @@
       </c>
       <c r="G22" s="49">
         <f>Tasks!Z21</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -14467,7 +14569,7 @@
       </c>
       <c r="G23" s="49">
         <f>Tasks!Z22</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -14493,7 +14595,7 @@
       </c>
       <c r="G24" s="49">
         <f>Tasks!Z23</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -14597,7 +14699,7 @@
       </c>
       <c r="G28" s="49">
         <f>Tasks!Z27</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -14623,7 +14725,7 @@
       </c>
       <c r="G29" s="49">
         <f>Tasks!Z28</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -14649,7 +14751,7 @@
       </c>
       <c r="G30" s="49">
         <f>Tasks!Z29</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -14675,7 +14777,7 @@
       </c>
       <c r="G31" s="49">
         <f>Tasks!Z30</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -14779,7 +14881,7 @@
       </c>
       <c r="G35" s="49">
         <f>Tasks!Z34</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -14805,7 +14907,7 @@
       </c>
       <c r="G36" s="49">
         <f>Tasks!Z35</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -14831,7 +14933,7 @@
       </c>
       <c r="G37" s="49">
         <f>Tasks!Z36</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -14883,7 +14985,7 @@
       </c>
       <c r="G39" s="49">
         <f>Tasks!Z38</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -14909,7 +15011,7 @@
       </c>
       <c r="G40" s="49">
         <f>Tasks!Z39</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -14935,7 +15037,7 @@
       </c>
       <c r="G41" s="49">
         <f>Tasks!Z40</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -14961,7 +15063,7 @@
       </c>
       <c r="G42" s="49">
         <f>Tasks!Z41</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -14987,7 +15089,7 @@
       </c>
       <c r="G43" s="49">
         <f>Tasks!Z42</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -15039,7 +15141,7 @@
       </c>
       <c r="G45" s="49">
         <f>Tasks!Z44</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -15065,7 +15167,7 @@
       </c>
       <c r="G46" s="49">
         <f>Tasks!Z45</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -15091,7 +15193,7 @@
       </c>
       <c r="G47" s="49">
         <f>Tasks!Z46</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -15117,7 +15219,7 @@
       </c>
       <c r="G48" s="49">
         <f>Tasks!Z47</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -15169,7 +15271,7 @@
       </c>
       <c r="G50" s="49">
         <f>Tasks!Z49</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -15195,7 +15297,7 @@
       </c>
       <c r="G51" s="49">
         <f>Tasks!Z50</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -15793,7 +15895,7 @@
       </c>
       <c r="G74" s="49">
         <f>Tasks!Z73</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -15819,7 +15921,7 @@
       </c>
       <c r="G75" s="49">
         <f>Tasks!Z74</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -15845,7 +15947,7 @@
       </c>
       <c r="G76" s="49">
         <f>Tasks!Z75</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -15867,11 +15969,11 @@
       </c>
       <c r="F77" s="54">
         <f>Tasks!W76</f>
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="G77" s="49">
         <f>Tasks!Z76</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -15893,11 +15995,11 @@
       </c>
       <c r="F78" s="54">
         <f>Tasks!W77</f>
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="G78" s="49">
         <f>Tasks!Z77</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -15923,7 +16025,7 @@
       </c>
       <c r="G79" s="49">
         <f>Tasks!Z78</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -15949,7 +16051,7 @@
       </c>
       <c r="G80" s="49">
         <f>Tasks!Z79</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -15975,7 +16077,7 @@
       </c>
       <c r="G81" s="49">
         <f>Tasks!Z80</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -16001,7 +16103,7 @@
       </c>
       <c r="G82" s="49">
         <f>Tasks!Z81</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -16079,7 +16181,7 @@
       </c>
       <c r="G85" s="49">
         <f>Tasks!Z84</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -16097,15 +16199,15 @@
       </c>
       <c r="E86" s="54">
         <f>Tasks!V85</f>
-        <v>8</v>
-      </c>
-      <c r="F86" s="54" t="e">
+        <v>22</v>
+      </c>
+      <c r="F86" s="54">
         <f>Tasks!W85</f>
-        <v>#NUM!</v>
+        <v>2</v>
       </c>
       <c r="G86" s="49">
         <f>Tasks!Z85</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -16131,7 +16233,7 @@
       </c>
       <c r="G87" s="49">
         <f>Tasks!Z86</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -16183,7 +16285,7 @@
       </c>
       <c r="G89" s="49">
         <f>Tasks!Z88</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -16209,7 +16311,7 @@
       </c>
       <c r="G90" s="49">
         <f>Tasks!Z89</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -16235,7 +16337,7 @@
       </c>
       <c r="G91" s="49">
         <f>Tasks!Z90</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -16261,7 +16363,7 @@
       </c>
       <c r="G92" s="49">
         <f>Tasks!Z91</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -16287,7 +16389,7 @@
       </c>
       <c r="G93" s="49">
         <f>Tasks!Z92</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -16303,17 +16405,17 @@
         <f>Tasks!U93</f>
         <v>7</v>
       </c>
-      <c r="E94" s="54" t="e">
+      <c r="E94" s="54">
         <f>Tasks!V93</f>
-        <v>#NUM!</v>
+        <v>24</v>
       </c>
       <c r="F94" s="54">
         <f>Tasks!W93</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G94" s="49">
         <f>Tasks!Z93</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -16339,7 +16441,7 @@
       </c>
       <c r="G95" s="49">
         <f>Tasks!Z94</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -16355,9 +16457,9 @@
         <f>Tasks!U95</f>
         <v>7</v>
       </c>
-      <c r="E96" s="54" t="e">
+      <c r="E96" s="54">
         <f>Tasks!V95</f>
-        <v>#NUM!</v>
+        <v>36</v>
       </c>
       <c r="F96" s="54">
         <f>Tasks!W95</f>
@@ -16365,7 +16467,7 @@
       </c>
       <c r="G96" s="49">
         <f>Tasks!Z95</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -16391,7 +16493,7 @@
       </c>
       <c r="G97" s="49">
         <f>Tasks!Z96</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -16485,9 +16587,9 @@
         <f>Tasks!U100</f>
         <v>7</v>
       </c>
-      <c r="E101" s="54" t="e">
+      <c r="E101" s="54">
         <f>Tasks!V100</f>
-        <v>#NUM!</v>
+        <v>36</v>
       </c>
       <c r="F101" s="54">
         <f>Tasks!W100</f>
@@ -16495,7 +16597,7 @@
       </c>
       <c r="G101" s="49">
         <f>Tasks!Z100</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -16521,7 +16623,7 @@
       </c>
       <c r="G102" s="49">
         <f>Tasks!Z101</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -16573,7 +16675,7 @@
       </c>
       <c r="G104" s="49">
         <f>Tasks!Z103</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -16677,7 +16779,7 @@
       </c>
       <c r="G108" s="49">
         <f>Tasks!Z107</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -16703,7 +16805,7 @@
       </c>
       <c r="G109" s="49">
         <f>Tasks!Z108</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -16729,7 +16831,7 @@
       </c>
       <c r="G110" s="49">
         <f>Tasks!Z109</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -16781,7 +16883,7 @@
       </c>
       <c r="G112" s="49">
         <f>Tasks!Z111</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -16807,7 +16909,7 @@
       </c>
       <c r="G113" s="49">
         <f>Tasks!Z112</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -16833,7 +16935,7 @@
       </c>
       <c r="G114" s="49">
         <f>Tasks!Z113</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -16885,7 +16987,7 @@
       </c>
       <c r="G116" s="49">
         <f>Tasks!Z115</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -16911,7 +17013,7 @@
       </c>
       <c r="G117" s="49">
         <f>Tasks!Z116</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -16937,7 +17039,7 @@
       </c>
       <c r="G118" s="49">
         <f>Tasks!Z117</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -17353,7 +17455,7 @@
       </c>
       <c r="G134" s="49">
         <f>Tasks!Z133</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -17379,7 +17481,7 @@
       </c>
       <c r="G135" s="49">
         <f>Tasks!Z134</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -17405,7 +17507,7 @@
       </c>
       <c r="G136" s="49">
         <f>Tasks!Z135</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -17431,7 +17533,7 @@
       </c>
       <c r="G137" s="49">
         <f>Tasks!Z136</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -17457,7 +17559,7 @@
       </c>
       <c r="G138" s="49">
         <f>Tasks!Z137</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -17483,7 +17585,7 @@
       </c>
       <c r="G139" s="49">
         <f>Tasks!Z138</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -17509,7 +17611,7 @@
       </c>
       <c r="G140" s="49">
         <f>Tasks!Z139</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -17535,7 +17637,7 @@
       </c>
       <c r="G141" s="49">
         <f>Tasks!Z140</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -17561,7 +17663,7 @@
       </c>
       <c r="G142" s="49">
         <f>Tasks!Z141</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -18349,8 +18451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1AC45A0-EB3A-4D5D-BD47-C1C54A3E083F}">
   <dimension ref="A2:H26"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18640,12 +18742,24 @@
       <c r="B19">
         <v>9</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
+      <c r="C19" s="12">
+        <v>1</v>
+      </c>
+      <c r="D19" s="12">
+        <v>1</v>
+      </c>
+      <c r="E19" s="12">
+        <v>1</v>
+      </c>
+      <c r="F19" s="12">
+        <v>1</v>
+      </c>
+      <c r="G19" s="12">
+        <v>1</v>
+      </c>
+      <c r="H19" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
@@ -18654,12 +18768,24 @@
       <c r="B20">
         <v>10</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
+      <c r="C20" s="12">
+        <v>1</v>
+      </c>
+      <c r="D20" s="12">
+        <v>1</v>
+      </c>
+      <c r="E20" s="12">
+        <v>1</v>
+      </c>
+      <c r="F20" s="12">
+        <v>1</v>
+      </c>
+      <c r="G20" s="12">
+        <v>1</v>
+      </c>
+      <c r="H20" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
@@ -18668,12 +18794,24 @@
       <c r="B21">
         <v>11</v>
       </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
+      <c r="C21" s="12">
+        <v>1</v>
+      </c>
+      <c r="D21" s="12">
+        <v>0</v>
+      </c>
+      <c r="E21" s="12">
+        <v>0</v>
+      </c>
+      <c r="F21" s="12">
+        <v>1</v>
+      </c>
+      <c r="G21" s="12">
+        <v>1</v>
+      </c>
+      <c r="H21" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
@@ -18682,12 +18820,24 @@
       <c r="B22">
         <v>12</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
+      <c r="C22" s="12">
+        <v>1</v>
+      </c>
+      <c r="D22" s="12">
+        <v>1</v>
+      </c>
+      <c r="E22" s="12">
+        <v>1</v>
+      </c>
+      <c r="F22" s="12">
+        <v>1</v>
+      </c>
+      <c r="G22" s="12">
+        <v>1</v>
+      </c>
+      <c r="H22" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B23" s="26"/>
@@ -18698,27 +18848,27 @@
       </c>
       <c r="C26">
         <f t="shared" ref="C26:H26" si="0">SUM(C11:C23)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E26">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G26">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="H26">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -18730,8 +18880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5364E817-80B1-4483-B837-995D14BDF7B6}">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18819,45 +18969,45 @@
         <v>98</v>
       </c>
       <c r="C11" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="D11" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="E11" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="F11" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="G11" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="H11" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="J11" s="13" t="s">
         <v>98</v>
       </c>
       <c r="K11" s="25">
         <f>AVERAGE(C11:D11)</f>
-        <v>0.16600000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="L11" s="25">
         <f>AVERAGE(C11:E11)</f>
-        <v>0.16600000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="M11" s="25">
         <f>AVERAGE(C11:F11)</f>
-        <v>0.16600000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="N11" s="25">
         <f>AVERAGE(C11:G11)</f>
-        <v>0.16600000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="O11" s="25">
-        <f t="shared" ref="O11:O16" si="0">AVERAGE(C11:H11)</f>
-        <v>0.16600000000000001</v>
+        <f>AVERAGE(C11:H11)*1.2</f>
+        <v>0.18</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
@@ -18865,45 +19015,45 @@
         <v>99</v>
       </c>
       <c r="C12" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="D12" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="E12" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="F12" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="G12" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="H12" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="J12" s="13" t="s">
         <v>99</v>
       </c>
       <c r="K12" s="25">
         <f>AVERAGE(C12:D12)</f>
-        <v>0.16600000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="L12" s="25">
         <f>AVERAGE(C12:E12)</f>
-        <v>0.16600000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="M12" s="25">
         <f>AVERAGE(C12:F12)</f>
-        <v>0.16600000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="N12" s="25">
         <f>AVERAGE(C12:G12)</f>
-        <v>0.16600000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="O12" s="25">
-        <f t="shared" si="0"/>
-        <v>0.16600000000000001</v>
+        <f>AVERAGE(C12:H12)*1.2</f>
+        <v>0.18</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
@@ -18911,22 +19061,22 @@
         <v>29</v>
       </c>
       <c r="C13" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="D13" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="E13" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="F13" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="G13" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="H13" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="J13" s="13" t="s">
         <v>29</v>
@@ -18934,19 +19084,19 @@
       <c r="K13" s="25"/>
       <c r="L13" s="25">
         <f>AVERAGE(C13:E13)</f>
-        <v>0.16600000000000001</v>
+        <v>0.10000000000000002</v>
       </c>
       <c r="M13" s="25">
         <f>AVERAGE(C13:F13)</f>
-        <v>0.16600000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="N13" s="25">
         <f>AVERAGE(C13:G13)</f>
-        <v>0.16600000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="O13" s="25">
-        <f t="shared" si="0"/>
-        <v>0.16600000000000001</v>
+        <f t="shared" ref="O13:O16" si="0">AVERAGE(C13:H13)*1.2</f>
+        <v>0.11999999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
@@ -18954,22 +19104,22 @@
         <v>30</v>
       </c>
       <c r="C14" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="D14" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E14" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="F14" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="G14" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="H14" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="J14" s="13" t="s">
         <v>30</v>
@@ -18978,15 +19128,15 @@
       <c r="L14" s="25"/>
       <c r="M14" s="25">
         <f>AVERAGE(C14:F14)</f>
-        <v>0.16600000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="N14" s="25">
         <f>AVERAGE(C14:G14)</f>
-        <v>0.16600000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="O14" s="25">
         <f t="shared" si="0"/>
-        <v>0.16600000000000001</v>
+        <v>0.23999999999999996</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
@@ -18994,22 +19144,22 @@
         <v>66</v>
       </c>
       <c r="C15" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="D15" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E15" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="F15" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="G15" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="H15" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="J15" s="13" t="s">
         <v>66</v>
@@ -19019,11 +19169,11 @@
       <c r="M15" s="25"/>
       <c r="N15" s="25">
         <f>AVERAGE(C15:G15)</f>
-        <v>0.16600000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="O15" s="25">
         <f t="shared" si="0"/>
-        <v>0.16600000000000001</v>
+        <v>0.23999999999999996</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
@@ -19031,22 +19181,22 @@
         <v>67</v>
       </c>
       <c r="C16" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="D16" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E16" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="F16" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="G16" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="H16" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="J16" s="13" t="s">
         <v>67</v>
@@ -19057,7 +19207,7 @@
       <c r="N16" s="25"/>
       <c r="O16" s="25">
         <f t="shared" si="0"/>
-        <v>0.16600000000000001</v>
+        <v>0.23999999999999996</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.35">
@@ -19065,28 +19215,28 @@
         <v>36</v>
       </c>
       <c r="C19">
-        <f t="shared" ref="C19:H19" si="1">SUM(C11:C16)</f>
-        <v>0.99600000000000011</v>
+        <f>SUM(C11:C16)</f>
+        <v>1</v>
       </c>
       <c r="D19">
-        <f t="shared" si="1"/>
-        <v>0.99600000000000011</v>
+        <f>SUM(D11:D16)</f>
+        <v>1</v>
       </c>
       <c r="E19">
-        <f t="shared" si="1"/>
-        <v>0.99600000000000011</v>
+        <f>SUM(E11:E16)</f>
+        <v>1</v>
       </c>
       <c r="F19">
-        <f t="shared" si="1"/>
-        <v>0.99600000000000011</v>
+        <f>SUM(F11:F16)</f>
+        <v>1</v>
       </c>
       <c r="G19">
-        <f t="shared" si="1"/>
-        <v>0.99600000000000011</v>
+        <f>SUM(G11:G16)</f>
+        <v>1</v>
       </c>
       <c r="H19">
-        <f t="shared" si="1"/>
-        <v>0.99600000000000011</v>
+        <f>SUM(H11:H16)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -19098,8 +19248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{861C5F3C-2BB8-48C2-B1E4-E1F141881B60}">
   <dimension ref="A1:Q81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="J68" sqref="J68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19229,8 +19379,8 @@
         <v>96</v>
       </c>
       <c r="B21" s="15">
-        <f>Tasks!B151</f>
-        <v>20</v>
+        <f>Tasks!B151+200</f>
+        <v>1075</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.35">
@@ -19270,7 +19420,7 @@
       </c>
       <c r="B27" s="25">
         <f>B21*B24+B22*B25</f>
-        <v>20</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.35">
@@ -19279,7 +19429,7 @@
       </c>
       <c r="B30">
         <f>Summary!B40</f>
-        <v>9.0909090909090917</v>
+        <v>8.3333333333333339</v>
       </c>
       <c r="M30" s="13"/>
       <c r="N30" s="13"/>
@@ -19302,7 +19452,7 @@
       </c>
       <c r="B33">
         <f>Summary!$B$39-Attendance!C26</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L33" s="13"/>
     </row>
@@ -19312,7 +19462,7 @@
       </c>
       <c r="B34">
         <f>Summary!$B$39-Attendance!D26</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L34" s="13"/>
     </row>
@@ -19322,7 +19472,7 @@
       </c>
       <c r="B35">
         <f>Summary!$B$39-Attendance!E26</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L35" s="13"/>
     </row>
@@ -19332,7 +19482,7 @@
       </c>
       <c r="B36">
         <f>Summary!$B$39-Attendance!F26</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L36" s="13"/>
     </row>
@@ -19342,7 +19492,7 @@
       </c>
       <c r="B37">
         <f>Summary!$B$39-Attendance!G26</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
@@ -19351,7 +19501,7 @@
       </c>
       <c r="B38">
         <f>Summary!$B$39-Attendance!H26</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.35">
@@ -19365,7 +19515,7 @@
       </c>
       <c r="B41">
         <f>-1*B33*Summary!$B$40</f>
-        <v>-36.363636363636367</v>
+        <v>-8.3333333333333339</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.35">
@@ -19374,7 +19524,7 @@
       </c>
       <c r="B42">
         <f>-1*B34*Summary!$B$40</f>
-        <v>-45.45454545454546</v>
+        <v>-25</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.35">
@@ -19383,7 +19533,7 @@
       </c>
       <c r="B43">
         <f>-1*B35*Summary!$B$40</f>
-        <v>-27.272727272727273</v>
+        <v>-8.3333333333333339</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.35">
@@ -19392,7 +19542,7 @@
       </c>
       <c r="B44">
         <f>-1*B36*Summary!$B$40</f>
-        <v>-27.272727272727273</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.35">
@@ -19401,7 +19551,7 @@
       </c>
       <c r="B45">
         <f>-1*B37*Summary!$B$40</f>
-        <v>-27.272727272727273</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.35">
@@ -19410,7 +19560,7 @@
       </c>
       <c r="B46">
         <f>-1*B38*Summary!$B$40</f>
-        <v>-27.272727272727273</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.35">
@@ -19494,23 +19644,23 @@
       </c>
       <c r="B58">
         <f>$B$27*'Effort %'!K11</f>
-        <v>3.3200000000000003</v>
+        <v>161.25</v>
       </c>
       <c r="C58">
         <f>$B$27*'Effort %'!L11</f>
-        <v>3.3200000000000003</v>
+        <v>161.25</v>
       </c>
       <c r="D58">
         <f>$B$27*'Effort %'!M11</f>
-        <v>3.3200000000000003</v>
+        <v>161.25</v>
       </c>
       <c r="E58">
         <f>$B$27*'Effort %'!N11</f>
-        <v>3.3200000000000003</v>
+        <v>161.25</v>
       </c>
       <c r="F58">
         <f>$B$27*'Effort %'!O11</f>
-        <v>3.3200000000000003</v>
+        <v>193.5</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
@@ -19519,23 +19669,23 @@
       </c>
       <c r="B59">
         <f>$B$27*'Effort %'!K12</f>
-        <v>3.3200000000000003</v>
+        <v>161.25</v>
       </c>
       <c r="C59">
         <f>$B$27*'Effort %'!L12</f>
-        <v>3.3200000000000003</v>
+        <v>161.25</v>
       </c>
       <c r="D59">
         <f>$B$27*'Effort %'!M12</f>
-        <v>3.3200000000000003</v>
+        <v>161.25</v>
       </c>
       <c r="E59">
         <f>$B$27*'Effort %'!N12</f>
-        <v>3.3200000000000003</v>
+        <v>161.25</v>
       </c>
       <c r="F59">
         <f>$B$27*'Effort %'!O12</f>
-        <v>3.3200000000000003</v>
+        <v>193.5</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
@@ -19548,19 +19698,19 @@
       </c>
       <c r="C60">
         <f>$B$27*'Effort %'!L13</f>
-        <v>3.3200000000000003</v>
+        <v>107.50000000000001</v>
       </c>
       <c r="D60">
         <f>$B$27*'Effort %'!M13</f>
-        <v>3.3200000000000003</v>
+        <v>107.5</v>
       </c>
       <c r="E60">
         <f>$B$27*'Effort %'!N13</f>
-        <v>3.3200000000000003</v>
+        <v>107.5</v>
       </c>
       <c r="F60">
         <f>$B$27*'Effort %'!O13</f>
-        <v>3.3200000000000003</v>
+        <v>128.99999999999997</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
@@ -19577,15 +19727,15 @@
       </c>
       <c r="D61">
         <f>$B$27*'Effort %'!M14</f>
-        <v>3.3200000000000003</v>
+        <v>215</v>
       </c>
       <c r="E61">
         <f>$B$27*'Effort %'!N14</f>
-        <v>3.3200000000000003</v>
+        <v>215</v>
       </c>
       <c r="F61">
         <f>$B$27*'Effort %'!O14</f>
-        <v>3.3200000000000003</v>
+        <v>257.99999999999994</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
@@ -19606,11 +19756,11 @@
       </c>
       <c r="E62">
         <f>$B$27*'Effort %'!N15</f>
-        <v>3.3200000000000003</v>
+        <v>215</v>
       </c>
       <c r="F62">
         <f>$B$27*'Effort %'!O15</f>
-        <v>3.3200000000000003</v>
+        <v>257.99999999999994</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
@@ -19635,7 +19785,7 @@
       </c>
       <c r="F63">
         <f>$B$27*'Effort %'!O16</f>
-        <v>3.3200000000000003</v>
+        <v>257.99999999999994</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
@@ -19656,11 +19806,11 @@
       </c>
       <c r="E66">
         <f>Summary!B47</f>
-        <v>303.75</v>
+        <v>243</v>
       </c>
       <c r="F66">
         <f>Summary!B48</f>
-        <v>364.5</v>
+        <v>243</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
@@ -19689,23 +19839,23 @@
       </c>
       <c r="B68">
         <f>MAX(0,MIN(100,B58/B$66*100))</f>
-        <v>1.366255144032922</v>
+        <v>66.358024691358025</v>
       </c>
       <c r="C68">
         <f>MAX(0,MIN(100,C58/C$66*100))</f>
-        <v>1.366255144032922</v>
+        <v>66.358024691358025</v>
       </c>
       <c r="D68">
         <f>MAX(0,MIN(100,D58/D$66*100))</f>
-        <v>1.366255144032922</v>
+        <v>66.358024691358025</v>
       </c>
       <c r="E68">
         <f>MAX(0,MIN(100,E58/E$66*100))</f>
-        <v>1.0930041152263374</v>
+        <v>66.358024691358025</v>
       </c>
       <c r="F68">
         <f>MAX(0,MIN(100,F58/F$66*100))</f>
-        <v>0.91083676268861469</v>
+        <v>79.629629629629633</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
@@ -19714,23 +19864,23 @@
       </c>
       <c r="B69">
         <f t="shared" ref="B69:F73" si="0">MAX(0,MIN(100,B59/B$66*100))</f>
-        <v>1.366255144032922</v>
+        <v>66.358024691358025</v>
       </c>
       <c r="C69">
         <f t="shared" si="0"/>
-        <v>1.366255144032922</v>
+        <v>66.358024691358025</v>
       </c>
       <c r="D69">
         <f t="shared" si="0"/>
-        <v>1.366255144032922</v>
+        <v>66.358024691358025</v>
       </c>
       <c r="E69">
         <f t="shared" si="0"/>
-        <v>1.0930041152263374</v>
+        <v>66.358024691358025</v>
       </c>
       <c r="F69">
         <f t="shared" si="0"/>
-        <v>0.91083676268861469</v>
+        <v>79.629629629629633</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
@@ -19743,19 +19893,19 @@
       </c>
       <c r="C70">
         <f t="shared" si="0"/>
-        <v>1.366255144032922</v>
+        <v>44.238683127572017</v>
       </c>
       <c r="D70">
         <f t="shared" si="0"/>
-        <v>1.366255144032922</v>
+        <v>44.238683127572017</v>
       </c>
       <c r="E70">
         <f t="shared" si="0"/>
-        <v>1.0930041152263374</v>
+        <v>44.238683127572017</v>
       </c>
       <c r="F70">
         <f t="shared" si="0"/>
-        <v>0.91083676268861469</v>
+        <v>53.08641975308641</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
@@ -19772,15 +19922,15 @@
       </c>
       <c r="D71">
         <f t="shared" si="0"/>
-        <v>1.366255144032922</v>
+        <v>88.477366255144034</v>
       </c>
       <c r="E71">
         <f t="shared" si="0"/>
-        <v>1.0930041152263374</v>
+        <v>88.477366255144034</v>
       </c>
       <c r="F71">
         <f t="shared" si="0"/>
-        <v>0.91083676268861469</v>
+        <v>100</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
@@ -19801,11 +19951,11 @@
       </c>
       <c r="E72">
         <f t="shared" si="0"/>
-        <v>1.0930041152263374</v>
+        <v>88.477366255144034</v>
       </c>
       <c r="F72">
         <f t="shared" si="0"/>
-        <v>0.91083676268861469</v>
+        <v>100</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
@@ -19830,7 +19980,7 @@
       </c>
       <c r="F73">
         <f t="shared" si="0"/>
-        <v>0.91083676268861469</v>
+        <v>100</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
@@ -19859,23 +20009,23 @@
       </c>
       <c r="B76" s="37">
         <f>MAX(0,MIN(100,B68+$B49+$B41))</f>
-        <v>0</v>
+        <v>83.024691358024697</v>
       </c>
       <c r="C76" s="37">
         <f>MAX(0,MIN(100,C68+$B49+$B41))</f>
-        <v>0</v>
+        <v>83.024691358024697</v>
       </c>
       <c r="D76" s="37">
         <f>MAX(0,MIN(100,D68+$B49+$B41))</f>
-        <v>0</v>
+        <v>83.024691358024697</v>
       </c>
       <c r="E76" s="37">
         <f>MAX(0,MIN(100,E68+$B49+$B41))</f>
-        <v>0</v>
+        <v>83.024691358024697</v>
       </c>
       <c r="F76" s="37">
         <f>MAX(0,MIN(100,F68+$B49+$B41))</f>
-        <v>0</v>
+        <v>96.296296296296305</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.35">
@@ -19884,23 +20034,23 @@
       </c>
       <c r="B77" s="37">
         <f>MAX(0,MIN(100,B69+$B50+$B42))</f>
-        <v>0</v>
+        <v>66.358024691358025</v>
       </c>
       <c r="C77" s="37">
         <f t="shared" ref="C77:F81" si="1">MAX(0,MIN(100,C69+$B50+$B42))</f>
-        <v>0</v>
+        <v>66.358024691358025</v>
       </c>
       <c r="D77" s="37">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>66.358024691358025</v>
       </c>
       <c r="E77" s="37">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>66.358024691358025</v>
       </c>
       <c r="F77" s="37">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79.629629629629633</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.35">
@@ -19910,19 +20060,19 @@
       <c r="B78" s="37"/>
       <c r="C78" s="37">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>35.905349794238681</v>
       </c>
       <c r="D78" s="37">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>35.905349794238681</v>
       </c>
       <c r="E78" s="37">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>35.905349794238681</v>
       </c>
       <c r="F78" s="37">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>44.753086419753075</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.35">
@@ -19933,15 +20083,15 @@
       <c r="C79" s="37"/>
       <c r="D79" s="37">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>88.477366255144034</v>
       </c>
       <c r="E79" s="37">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>88.477366255144034</v>
       </c>
       <c r="F79" s="37">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.35">
@@ -19953,11 +20103,11 @@
       <c r="D80" s="37"/>
       <c r="E80" s="37">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>88.477366255144034</v>
       </c>
       <c r="F80" s="37">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.35">
@@ -19970,7 +20120,7 @@
       <c r="E81" s="37"/>
       <c r="F81" s="37">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -19979,6 +20129,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100425D870C9FE3FA459BE7BAB817912A28" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2888a6b5c62326ad14675b6ae20d83ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="19dc0929-3265-432c-90cd-a4a18b147cbc" xmlns:ns4="e15c2e9d-9071-420f-8402-443b554f1232" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="df22a33983a74acd15e217796b17182e" ns3:_="" ns4:_="">
     <xsd:import namespace="19dc0929-3265-432c-90cd-a4a18b147cbc"/>
@@ -20225,15 +20384,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -20243,6 +20393,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75E4E88A-17F8-40B2-8EC1-AE408CF7AA54}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F9BD7DA-52C8-49CE-B9E2-21F98F087543}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20257,14 +20415,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75E4E88A-17F8-40B2-8EC1-AE408CF7AA54}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>